<commit_message>
Nettoyage de la documentation utilisateur
</commit_message>
<xml_diff>
--- a/FichesTemps/MaximeAubin5.xlsx
+++ b/FichesTemps/MaximeAubin5.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BC76B77-872D-4D9F-B475-A0862A9B8363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AD59FC-53BB-467C-BBBF-511754081FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="bsnEa0N1OcI6znPoPEcq3AHEi57LtmD/hoPfLk9LAHbO8ZgF/KxDU64xoRN551lSOgXhKiKNTKiOVsg9sOO7CQ==" workbookSaltValue="Arsw55Oy1Kl5wQ7vU+yWcQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="91">
   <si>
     <t>Fiche d'évaluation du travail d'équipe</t>
   </si>
@@ -398,6 +398,27 @@
   </si>
   <si>
     <t>Rencontre pour stages en classe</t>
+  </si>
+  <si>
+    <t>Rencontre d'équipe</t>
+  </si>
+  <si>
+    <t>Évaluation des compétences</t>
+  </si>
+  <si>
+    <t>Révision du projet</t>
+  </si>
+  <si>
+    <t>21/02/2023</t>
+  </si>
+  <si>
+    <t>Fix bug Yarn.lock qui empêchait de build</t>
+  </si>
+  <si>
+    <t>Modification de la documentation pour utilisateur pour inclure les informations sur les derniers changements</t>
+  </si>
+  <si>
+    <t>Correction et nettoyage de la documentation pour utilisateur</t>
   </si>
 </sst>
 </file>
@@ -1796,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B1E992-A4D6-4269-AA92-453ABD10AC9B}">
   <dimension ref="A1:F466"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1890,7 +1911,7 @@
       </c>
       <c r="C9" s="47">
         <f>SUM(C11:C466)</f>
-        <v>0.5</v>
+        <v>12</v>
       </c>
       <c r="D9" s="46" t="s">
         <v>64</v>
@@ -1926,22 +1947,40 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="48"/>
+      <c r="A12" s="48" t="s">
+        <v>82</v>
+      </c>
       <c r="B12" s="52"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="52"/>
+      <c r="C12" s="53">
+        <v>1</v>
+      </c>
+      <c r="D12" s="52" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="48"/>
+      <c r="A13" s="48" t="s">
+        <v>82</v>
+      </c>
       <c r="B13" s="52"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="52"/>
+      <c r="C13" s="53">
+        <v>1</v>
+      </c>
+      <c r="D13" s="52" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="48"/>
+      <c r="A14" s="48" t="s">
+        <v>82</v>
+      </c>
       <c r="B14" s="52"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="52"/>
+      <c r="C14" s="53">
+        <v>3</v>
+      </c>
+      <c r="D14" s="52" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="48"/>
@@ -1950,28 +1989,52 @@
       <c r="D15" s="52"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="48"/>
+      <c r="A16" s="48" t="s">
+        <v>87</v>
+      </c>
       <c r="B16" s="52"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="52"/>
+      <c r="C16" s="53">
+        <v>3</v>
+      </c>
+      <c r="D16" s="52" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="48"/>
+      <c r="A17" s="48" t="s">
+        <v>87</v>
+      </c>
       <c r="B17" s="52"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="52"/>
+      <c r="C17" s="53">
+        <v>1</v>
+      </c>
+      <c r="D17" s="52" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="48"/>
+      <c r="A18" s="48" t="s">
+        <v>87</v>
+      </c>
       <c r="B18" s="52"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="52"/>
+      <c r="C18" s="53">
+        <v>1.5</v>
+      </c>
+      <c r="D18" s="52" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="48"/>
+      <c r="A19" s="48" t="s">
+        <v>87</v>
+      </c>
       <c r="B19" s="52"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="52"/>
+      <c r="C19" s="53">
+        <v>1</v>
+      </c>
+      <c r="D19" s="52" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="48"/>

</xml_diff>